<commit_message>
poller is working, added the needed libraries to the deploy script
</commit_message>
<xml_diff>
--- a/poll/influxdb data.xlsx
+++ b/poll/influxdb data.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="1820" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>time of measurement</t>
   </si>
@@ -87,18 +87,9 @@
     <t>Mesowest</t>
   </si>
   <si>
-    <t>timestamp</t>
-  </si>
-  <si>
     <t>MAC address</t>
   </si>
   <si>
-    <t>????</t>
-  </si>
-  <si>
-    <t>Is time of registration and start not very similar??</t>
-  </si>
-  <si>
     <t>Sensor Source (DAQ, Mesowest, ours or Purple Air)</t>
   </si>
   <si>
@@ -108,9 +99,6 @@
     <t>wind speed (scalar)</t>
   </si>
   <si>
-    <t>self assigned ID</t>
-  </si>
-  <si>
     <t>AirU (ours)</t>
   </si>
   <si>
@@ -126,13 +114,16 @@
     <t>solar radiation</t>
   </si>
   <si>
-    <t>wind_gust</t>
-  </si>
-  <si>
     <t>tag</t>
   </si>
   <si>
     <t>field</t>
+  </si>
+  <si>
+    <t>wind gust</t>
+  </si>
+  <si>
+    <t>name</t>
   </si>
 </sst>
 </file>
@@ -225,7 +216,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -233,8 +224,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -248,9 +245,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -267,14 +261,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -604,10 +608,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -621,26 +625,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="11" t="s">
-        <v>36</v>
+      <c r="A1" s="10" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="12" t="s">
-        <v>37</v>
+      <c r="A2" s="11" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="B3" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="13" t="s">
+      <c r="B3" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" s="13" t="s">
+      <c r="D3" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="12" t="s">
         <v>21</v>
       </c>
     </row>
@@ -650,115 +654,122 @@
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="11" t="s">
-        <v>13</v>
+      <c r="A5" s="10" t="s">
+        <v>1</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>22</v>
       </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>23</v>
-      </c>
+      <c r="A6" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="4"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="11" t="s">
-        <v>14</v>
+      <c r="A7" s="10" t="s">
+        <v>15</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="11" t="s">
-        <v>15</v>
+      <c r="A8" s="10" t="s">
+        <v>16</v>
       </c>
       <c r="B8" s="4"/>
-      <c r="C8" s="5"/>
+      <c r="C8" s="6"/>
       <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="11" t="s">
-        <v>16</v>
+      <c r="A9" s="10" t="s">
+        <v>17</v>
       </c>
       <c r="B9" s="4"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="5"/>
+      <c r="C9" s="5"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="11" t="s">
-        <v>17</v>
+      <c r="A10" s="10" t="s">
+        <v>18</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="5"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="4"/>
+      <c r="A11" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="C11" s="5"/>
+      <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>24</v>
-      </c>
+      <c r="A12" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="7"/>
       <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="11" t="s">
-        <v>26</v>
-      </c>
       <c r="B13" s="8"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="B14" s="9"/>
+      <c r="B14" s="8"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="B15" s="9"/>
+      <c r="B15" s="8"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="B16" s="9"/>
+      <c r="A16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="8"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17" s="9"/>
+      <c r="A17" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="12" t="s">
-        <v>0</v>
+      <c r="A18" s="11" t="s">
+        <v>2</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="11" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B19" s="4"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="4" t="s">
-        <v>29</v>
-      </c>
+      <c r="D19" s="9"/>
+      <c r="E19" s="5"/>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="12" t="s">
-        <v>2</v>
+      <c r="A20" s="11" t="s">
+        <v>4</v>
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="5"/>
@@ -766,16 +777,15 @@
       <c r="E20" s="5"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="12" t="s">
-        <v>3</v>
+      <c r="A21" s="11" t="s">
+        <v>5</v>
       </c>
       <c r="B21" s="4"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="5"/>
+      <c r="C21" s="5"/>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="12" t="s">
-        <v>4</v>
+      <c r="A22" s="11" t="s">
+        <v>6</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="5"/>
@@ -783,63 +793,63 @@
       <c r="E22" s="5"/>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="12" t="s">
-        <v>5</v>
+      <c r="A23" s="11" t="s">
+        <v>7</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="12" t="s">
-        <v>6</v>
+      <c r="A24" s="11" t="s">
+        <v>8</v>
       </c>
       <c r="B24" s="4"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="12" t="s">
-        <v>7</v>
+      <c r="A25" s="11" t="s">
+        <v>9</v>
       </c>
       <c r="B25" s="4"/>
-      <c r="C25" s="5"/>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="12" t="s">
-        <v>8</v>
+      <c r="A26" s="11" t="s">
+        <v>10</v>
       </c>
       <c r="B26" s="4"/>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B27" s="4"/>
+      <c r="A27" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B28" s="4"/>
+      <c r="A28" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="D29" s="5"/>
+      <c r="A29" s="11" t="s">
+        <v>28</v>
+      </c>
       <c r="E29" s="5"/>
     </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
+    <row r="30" spans="1:5" s="14" customFormat="1">
+      <c r="A30" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" s="13"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="12" t="s">
-        <v>32</v>
+      <c r="A31" s="11" t="s">
+        <v>30</v>
       </c>
       <c r="E31" s="5"/>
     </row>
@@ -848,23 +858,6 @@
         <v>33</v>
       </c>
       <c r="E32" s="5"/>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E33" s="5"/>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="E34" s="5"/>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="1" t="s">
-        <v>25</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
wind speed and gust is stored in m/s and not miles/hour
</commit_message>
<xml_diff>
--- a/poll/influxdb data.xlsx
+++ b/poll/influxdb data.xlsx
@@ -9,6 +9,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$E$32</definedName>
+  </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -130,7 +133,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -170,6 +173,12 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -611,7 +620,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection sqref="A1:E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -860,8 +869,9 @@
       <c r="E32" s="5"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup scale="83" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>